<commit_message>
CE06ISSP Cal and Ingest CSV
removed m from depth value
</commit_message>
<xml_diff>
--- a/CE06ISSP/Omaha_Cal_Info_CE06ISSP_00001.xlsx
+++ b/CE06ISSP/Omaha_Cal_Info_CE06ISSP_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="840" windowWidth="25600" windowHeight="16060" tabRatio="579" activeTab="1"/>
+    <workbookView xWindow="855" yWindow="840" windowWidth="25605" windowHeight="16065" tabRatio="579"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$G$51</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
   <si>
     <t>Ref Des</t>
   </si>
@@ -345,9 +345,6 @@
     <t>47° 8.0880' N</t>
   </si>
   <si>
-    <t>29 m</t>
-  </si>
-  <si>
     <t>Endurance III</t>
   </si>
   <si>
@@ -362,10 +359,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="36" x14ac:knownFonts="1">
     <font>
@@ -601,6 +598,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -714,14 +712,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1249,7 +1247,7 @@
     <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1268,10 +1266,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1340,7 +1338,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1889,7 +1887,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -2229,28 +2227,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="28">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2273,7 +2271,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>32</v>
@@ -2285,7 +2283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>64</v>
       </c>
@@ -2308,13 +2306,13 @@
         <v>99</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="44">
+        <v>29</v>
+      </c>
+      <c r="J2" s="44" t="s">
         <v>100</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>101</v>
       </c>
       <c r="L2" s="8">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
@@ -2325,25 +2323,25 @@
         <v>-124.27325999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="9" customFormat="1">
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:13" s="9" customFormat="1">
+    <row r="4" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="1:13" s="9" customFormat="1">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:13" s="9" customFormat="1">
+    <row r="6" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
@@ -2352,7 +2350,7 @@
         <v>47.134799999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="9" customFormat="1">
+    <row r="7" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
@@ -2361,61 +2359,61 @@
         <v>-124.27325999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="9" customFormat="1">
+    <row r="8" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:13" s="9" customFormat="1">
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:13" s="9" customFormat="1">
+    <row r="10" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:13" s="9" customFormat="1">
+    <row r="11" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1">
+    <row r="12" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:13" s="9" customFormat="1">
+    <row r="13" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:13" s="9" customFormat="1">
+    <row r="14" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:13" s="9" customFormat="1">
+    <row r="15" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:13" s="9" customFormat="1">
+    <row r="16" spans="1:13" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="3:6" s="9" customFormat="1">
+    <row r="17" spans="3:6" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
@@ -2439,22 +2437,22 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -2486,7 +2484,7 @@
       <c r="F2" s="20"/>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1">
+    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>68</v>
       </c>
@@ -2509,7 +2507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1">
+    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>68</v>
       </c>
@@ -2532,7 +2530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" ht="15">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>68</v>
       </c>
@@ -2555,7 +2553,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>68</v>
       </c>
@@ -2578,7 +2576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="7" customFormat="1">
+    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
@@ -2587,7 +2585,7 @@
       <c r="F7" s="25"/>
       <c r="G7" s="20"/>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1">
+    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>67</v>
       </c>
@@ -2610,7 +2608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>67</v>
       </c>
@@ -2631,7 +2629,7 @@
       </c>
       <c r="G9" s="31"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>67</v>
       </c>
@@ -2652,7 +2650,7 @@
       </c>
       <c r="G10" s="31"/>
     </row>
-    <row r="11" spans="1:7" s="7" customFormat="1">
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>67</v>
       </c>
@@ -2673,7 +2671,7 @@
       </c>
       <c r="G11" s="31"/>
     </row>
-    <row r="12" spans="1:7" s="7" customFormat="1">
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>67</v>
       </c>
@@ -2694,7 +2692,7 @@
       </c>
       <c r="G12" s="31"/>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1">
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>67</v>
       </c>
@@ -2715,7 +2713,7 @@
       </c>
       <c r="G13" s="31"/>
     </row>
-    <row r="14" spans="1:7" s="7" customFormat="1">
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>67</v>
       </c>
@@ -2736,7 +2734,7 @@
       </c>
       <c r="G14" s="31"/>
     </row>
-    <row r="15" spans="1:7" s="7" customFormat="1">
+    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>67</v>
       </c>
@@ -2757,7 +2755,7 @@
       </c>
       <c r="G15" s="31"/>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1">
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
@@ -2766,7 +2764,7 @@
       <c r="F16" s="25"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="1:7" s="7" customFormat="1">
+    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>69</v>
       </c>
@@ -2789,7 +2787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1">
+    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>69</v>
       </c>
@@ -2812,7 +2810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1">
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="27"/>
       <c r="C19" s="28"/>
@@ -2821,7 +2819,7 @@
       <c r="F19" s="25"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1">
+    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>70</v>
       </c>
@@ -2844,7 +2842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1">
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>70</v>
       </c>
@@ -2867,7 +2865,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1">
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>70</v>
       </c>
@@ -2890,7 +2888,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>70</v>
       </c>
@@ -2913,7 +2911,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="7" customFormat="1">
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>70</v>
       </c>
@@ -2936,7 +2934,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="7" customFormat="1">
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>70</v>
       </c>
@@ -2959,7 +2957,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1">
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>70</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1">
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -2991,7 +2989,7 @@
       <c r="F27" s="25"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
         <v>71</v>
       </c>
@@ -3012,7 +3010,7 @@
       </c>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1">
+    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>71</v>
       </c>
@@ -3033,7 +3031,7 @@
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>71</v>
       </c>
@@ -3054,7 +3052,7 @@
       </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1">
+    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="27"/>
       <c r="C31" s="28"/>
@@ -3063,7 +3061,7 @@
       <c r="F31" s="25"/>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1">
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>72</v>
       </c>
@@ -3086,7 +3084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="7" customFormat="1">
+    <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
         <v>72</v>
       </c>
@@ -3109,7 +3107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="7" customFormat="1">
+    <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>72</v>
       </c>
@@ -3132,7 +3130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="7" customFormat="1">
+    <row r="35" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
         <v>72</v>
       </c>
@@ -3155,7 +3153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="7" customFormat="1">
+    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>72</v>
       </c>
@@ -3178,7 +3176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="7" customFormat="1">
+    <row r="37" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>72</v>
       </c>
@@ -3201,7 +3199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="7" customFormat="1">
+    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>72</v>
       </c>
@@ -3224,7 +3222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1">
+    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>72</v>
       </c>
@@ -3247,7 +3245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1">
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>72</v>
       </c>
@@ -3270,7 +3268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="7" customFormat="1">
+    <row r="41" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
         <v>72</v>
       </c>
@@ -3293,7 +3291,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="7" customFormat="1">
+    <row r="42" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -3302,7 +3300,7 @@
       <c r="F42" s="25"/>
       <c r="G42" s="20"/>
     </row>
-    <row r="43" spans="1:7" s="7" customFormat="1">
+    <row r="43" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>73</v>
       </c>
@@ -3325,7 +3323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="7" customFormat="1">
+    <row r="44" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>73</v>
       </c>
@@ -3348,7 +3346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="7" customFormat="1">
+    <row r="45" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="27"/>
       <c r="C45" s="28"/>
@@ -3357,7 +3355,7 @@
       <c r="F45" s="25"/>
       <c r="G45" s="20"/>
     </row>
-    <row r="46" spans="1:7" s="7" customFormat="1">
+    <row r="46" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>74</v>
       </c>
@@ -3378,7 +3376,7 @@
       </c>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="1:7" s="7" customFormat="1">
+    <row r="47" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
         <v>74</v>
       </c>
@@ -3399,7 +3397,7 @@
       </c>
       <c r="G47" s="20"/>
     </row>
-    <row r="48" spans="1:7" s="7" customFormat="1">
+    <row r="48" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
         <v>74</v>
       </c>
@@ -3420,7 +3418,7 @@
       </c>
       <c r="G48" s="20"/>
     </row>
-    <row r="49" spans="1:7" s="13" customFormat="1">
+    <row r="49" spans="1:7" s="13" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="33"/>
       <c r="C49" s="24"/>
@@ -3429,7 +3427,7 @@
       <c r="F49" s="34"/>
       <c r="G49" s="33"/>
     </row>
-    <row r="50" spans="1:7" s="7" customFormat="1">
+    <row r="50" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>75</v>
       </c>
@@ -3446,10 +3444,10 @@
       <c r="F50" s="36"/>
       <c r="G50" s="20"/>
     </row>
-    <row r="51" spans="1:7" s="7" customFormat="1"/>
-    <row r="52" spans="1:7" s="7" customFormat="1"/>
-    <row r="53" spans="1:7" s="7" customFormat="1"/>
-    <row r="54" spans="1:7" s="7" customFormat="1"/>
+    <row r="51" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="34" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3470,9 +3468,9 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-2.5780999999999998E-2</v>
       </c>
@@ -3579,7 +3577,7 @@
         <v>2.1193E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1.7167999999999999E-2</v>
       </c>
@@ -3686,7 +3684,7 @@
         <v>1.1336000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-8.5559999999999994E-3</v>
       </c>
@@ -3793,7 +3791,7 @@
         <v>2.3340000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5.0000000000000002E-5</v>
       </c>
@@ -3900,7 +3898,7 @@
         <v>-4.3610000000000003E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.117E-3</v>
       </c>
@@ -4007,7 +4005,7 @@
         <v>-7.6249999999999998E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.182E-3</v>
       </c>
@@ -4114,7 +4112,7 @@
         <v>-9.7070000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.6540000000000002E-3</v>
       </c>
@@ -4221,7 +4219,7 @@
         <v>-1.0126E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.8370000000000001E-3</v>
       </c>
@@ -4328,7 +4326,7 @@
         <v>-9.5200000000000007E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.9389999999999998E-3</v>
       </c>
@@ -4435,7 +4433,7 @@
         <v>-9.9399999999999992E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.679E-3</v>
       </c>
@@ -4542,7 +4540,7 @@
         <v>-9.6399999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.9609999999999993E-3</v>
       </c>
@@ -4649,7 +4647,7 @@
         <v>-9.2029999999999994E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8.8800000000000007E-3</v>
       </c>
@@ -4756,7 +4754,7 @@
         <v>-8.9390000000000008E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9.4479999999999998E-3</v>
       </c>
@@ -4863,7 +4861,7 @@
         <v>-8.8070000000000006E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9.8200000000000006E-3</v>
       </c>
@@ -4970,7 +4968,7 @@
         <v>-8.3180000000000007E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.0178E-2</v>
       </c>
@@ -5077,7 +5075,7 @@
         <v>-8.3160000000000005E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.1164E-2</v>
       </c>
@@ -5184,7 +5182,7 @@
         <v>-7.9609999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.1211E-2</v>
       </c>
@@ -5291,7 +5289,7 @@
         <v>-7.6880000000000004E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.0957E-2</v>
       </c>
@@ -5398,7 +5396,7 @@
         <v>-7.3470000000000002E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.0567E-2</v>
       </c>
@@ -5505,7 +5503,7 @@
         <v>-7.0359999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9.6740000000000003E-3</v>
       </c>
@@ -5612,7 +5610,7 @@
         <v>-6.6239999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9.3410000000000003E-3</v>
       </c>
@@ -5719,7 +5717,7 @@
         <v>-6.306E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8.4539999999999997E-3</v>
       </c>
@@ -5826,7 +5824,7 @@
         <v>-5.8950000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8.2310000000000005E-3</v>
       </c>
@@ -5933,7 +5931,7 @@
         <v>-5.509E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7.3109999999999998E-3</v>
       </c>
@@ -6040,7 +6038,7 @@
         <v>-5.019E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6.7530000000000003E-3</v>
       </c>
@@ -6147,7 +6145,7 @@
         <v>-4.646E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6.3889999999999997E-3</v>
       </c>
@@ -6254,7 +6252,7 @@
         <v>-4.2750000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.8970000000000003E-3</v>
       </c>
@@ -6361,7 +6359,7 @@
         <v>-3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.5420000000000001E-3</v>
       </c>
@@ -6468,7 +6466,7 @@
         <v>-3.4640000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4.9880000000000002E-3</v>
       </c>
@@ -6575,7 +6573,7 @@
         <v>-3.1089999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4.999E-3</v>
       </c>
@@ -6682,7 +6680,7 @@
         <v>-2.807E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4.6410000000000002E-3</v>
       </c>
@@ -6789,7 +6787,7 @@
         <v>-2.444E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.5269999999999998E-3</v>
       </c>
@@ -6896,7 +6894,7 @@
         <v>-2.173E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.1970000000000002E-3</v>
       </c>
@@ -7003,7 +7001,7 @@
         <v>-1.92E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3.8089999999999999E-3</v>
       </c>
@@ -7110,7 +7108,7 @@
         <v>-1.7129999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3.189E-3</v>
       </c>
@@ -7217,7 +7215,7 @@
         <v>-1.567E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2.2560000000000002E-3</v>
       </c>
@@ -7324,7 +7322,7 @@
         <v>-1.438E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.147E-3</v>
       </c>
@@ -7431,7 +7429,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-4.4700000000000002E-4</v>
       </c>
@@ -7538,7 +7536,7 @@
         <v>-1.328E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-2.1570000000000001E-3</v>
       </c>
@@ -7645,7 +7643,7 @@
         <v>-1.4239999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-3.0799999999999998E-3</v>
       </c>
@@ -7752,7 +7750,7 @@
         <v>-1.467E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-3.5469999999999998E-3</v>
       </c>
@@ -7859,7 +7857,7 @@
         <v>-1.64E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-3.1150000000000001E-3</v>
       </c>
@@ -7966,7 +7964,7 @@
         <v>-1.7359999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-5.0340000000000003E-3</v>
       </c>
@@ -8073,7 +8071,7 @@
         <v>-7.4200000000000004E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-4.5750000000000001E-3</v>
       </c>
@@ -8180,7 +8178,7 @@
         <v>-7.5600000000000005E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-4.5779999999999996E-3</v>
       </c>
@@ -8287,7 +8285,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-4.176E-3</v>
       </c>
@@ -8394,7 +8392,7 @@
         <v>-7.2400000000000003E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-4.071E-3</v>
       </c>
@@ -8501,7 +8499,7 @@
         <v>-7.6000000000000004E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-3.8679999999999999E-3</v>
       </c>
@@ -8608,7 +8606,7 @@
         <v>-7.8799999999999996E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-3.5279999999999999E-3</v>
       </c>
@@ -8715,7 +8713,7 @@
         <v>-7.8100000000000001E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-3.3969999999999998E-3</v>
       </c>
@@ -8822,7 +8820,7 @@
         <v>-7.6999999999999996E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-3.4169999999999999E-3</v>
       </c>
@@ -8929,7 +8927,7 @@
         <v>-7.94E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-3.483E-3</v>
       </c>
@@ -9036,7 +9034,7 @@
         <v>-7.9100000000000004E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-3.454E-3</v>
       </c>
@@ -9143,7 +9141,7 @@
         <v>-7.2199999999999999E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3.4759999999999999E-3</v>
       </c>
@@ -9250,7 +9248,7 @@
         <v>-7.1699999999999997E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-3.5729999999999998E-3</v>
       </c>
@@ -9357,7 +9355,7 @@
         <v>-7.2000000000000005E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-3.666E-3</v>
       </c>
@@ -9464,7 +9462,7 @@
         <v>-6.5499999999999998E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-3.771E-3</v>
       </c>
@@ -9571,7 +9569,7 @@
         <v>-6.4599999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-3.8969999999999999E-3</v>
       </c>
@@ -9678,7 +9676,7 @@
         <v>-6.0800000000000003E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-4.0460000000000001E-3</v>
       </c>
@@ -9785,7 +9783,7 @@
         <v>-6.0599999999999998E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-4.1229999999999999E-3</v>
       </c>
@@ -9892,7 +9890,7 @@
         <v>-5.71E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-4.4140000000000004E-3</v>
       </c>
@@ -9999,7 +9997,7 @@
         <v>-5.0500000000000002E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-4.5139999999999998E-3</v>
       </c>
@@ -10106,7 +10104,7 @@
         <v>-4.6500000000000003E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-4.5279999999999999E-3</v>
       </c>
@@ -10213,7 +10211,7 @@
         <v>-4.3399999999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-4.7699999999999999E-3</v>
       </c>
@@ -10320,7 +10318,7 @@
         <v>-4.0299999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-4.6909999999999999E-3</v>
       </c>
@@ -10427,7 +10425,7 @@
         <v>-3.4900000000000003E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-4.9100000000000003E-3</v>
       </c>
@@ -10534,7 +10532,7 @@
         <v>-3.3E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-4.9040000000000004E-3</v>
       </c>
@@ -10641,7 +10639,7 @@
         <v>-3.1199999999999999E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-4.9459999999999999E-3</v>
       </c>
@@ -10748,7 +10746,7 @@
         <v>-3.1500000000000001E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-5.2160000000000002E-3</v>
       </c>
@@ -10855,7 +10853,7 @@
         <v>-2.9100000000000003E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-5.1619999999999999E-3</v>
       </c>
@@ -10962,7 +10960,7 @@
         <v>-2.5099999999999998E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-5.267E-3</v>
       </c>
@@ -11069,7 +11067,7 @@
         <v>-2.6899999999999998E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-5.3049999999999998E-3</v>
       </c>
@@ -11176,7 +11174,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-5.1419999999999999E-3</v>
       </c>
@@ -11283,7 +11281,7 @@
         <v>-2.6699999999999998E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-5.0359999999999997E-3</v>
       </c>
@@ -11390,7 +11388,7 @@
         <v>-1.83E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.3579999999999999E-3</v>
       </c>
@@ -11497,7 +11495,7 @@
         <v>-7.7999999999999999E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-5.3299999999999997E-3</v>
       </c>
@@ -11604,7 +11602,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="77" spans="1:35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-5.3070000000000001E-3</v>
       </c>
@@ -11711,7 +11709,7 @@
         <v>7.6000000000000004E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-5.2009999999999999E-3</v>
       </c>
@@ -11818,7 +11816,7 @@
         <v>1.05E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-4.8599999999999997E-3</v>
       </c>
@@ -11925,7 +11923,7 @@
         <v>1.8900000000000001E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-4.6449999999999998E-3</v>
       </c>
@@ -12032,7 +12030,7 @@
         <v>1.3899999999999999E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-4.365E-3</v>
       </c>
@@ -12139,7 +12137,7 @@
         <v>2.02E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-4.7549999999999997E-3</v>
       </c>
@@ -12246,7 +12244,7 @@
         <v>2.1100000000000001E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-4.6899999999999997E-3</v>
       </c>
@@ -12353,7 +12351,7 @@
         <v>3.3199999999999999E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-5.0220000000000004E-3</v>
       </c>
@@ -12460,7 +12458,7 @@
         <v>3.7100000000000002E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.5160000000000001E-3</v>
       </c>
@@ -12585,9 +12583,9 @@
       <selection sqref="A1:AI85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-4.1287999999999998E-2</v>
       </c>
@@ -12694,7 +12692,7 @@
         <v>-1.4790000000000001E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-4.1367000000000001E-2</v>
       </c>
@@ -12801,7 +12799,7 @@
         <v>-2.611E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-3.7718000000000002E-2</v>
       </c>
@@ -12908,7 +12906,7 @@
         <v>-1.418E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-3.5545E-2</v>
       </c>
@@ -13015,7 +13013,7 @@
         <v>-2.5010000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-3.0488999999999999E-2</v>
       </c>
@@ -13122,7 +13120,7 @@
         <v>-2.6819999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-2.7740999999999998E-2</v>
       </c>
@@ -13229,7 +13227,7 @@
         <v>-3.4970000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-2.4542999999999999E-2</v>
       </c>
@@ -13336,7 +13334,7 @@
         <v>-2.663E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-2.3806999999999998E-2</v>
       </c>
@@ -13443,7 +13441,7 @@
         <v>-3.852E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-2.1422E-2</v>
       </c>
@@ -13550,7 +13548,7 @@
         <v>-4.0220000000000004E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-2.0753000000000001E-2</v>
       </c>
@@ -13657,7 +13655,7 @@
         <v>-4.2459999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1.8873999999999998E-2</v>
       </c>
@@ -13764,7 +13762,7 @@
         <v>-3.9769999999999996E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-1.8828999999999999E-2</v>
       </c>
@@ -13871,7 +13869,7 @@
         <v>-4.2550000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-1.8471000000000001E-2</v>
       </c>
@@ -13978,7 +13976,7 @@
         <v>-4.2909999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1.7864000000000001E-2</v>
       </c>
@@ -14085,7 +14083,7 @@
         <v>-4.2659999999999998E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-1.7205000000000002E-2</v>
       </c>
@@ -14192,7 +14190,7 @@
         <v>-4.1949999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-1.7103E-2</v>
       </c>
@@ -14299,7 +14297,7 @@
         <v>-4.1640000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-1.6115999999999998E-2</v>
       </c>
@@ -14406,7 +14404,7 @@
         <v>-4.267E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-1.5507E-2</v>
       </c>
@@ -14513,7 +14511,7 @@
         <v>-4.1989999999999996E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-1.473E-2</v>
       </c>
@@ -14620,7 +14618,7 @@
         <v>-4.15E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-1.3806000000000001E-2</v>
       </c>
@@ -14727,7 +14725,7 @@
         <v>-4.0239999999999998E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-1.2939000000000001E-2</v>
       </c>
@@ -14834,7 +14832,7 @@
         <v>-4.0619999999999996E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-1.2475E-2</v>
       </c>
@@ -14941,7 +14939,7 @@
         <v>-3.9150000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-1.1646999999999999E-2</v>
       </c>
@@ -15048,7 +15046,7 @@
         <v>-3.954E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-1.0881E-2</v>
       </c>
@@ -15155,7 +15153,7 @@
         <v>-4.0109999999999998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>-1.0399E-2</v>
       </c>
@@ -15262,7 +15260,7 @@
         <v>-3.8639999999999998E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>-9.9030000000000003E-3</v>
       </c>
@@ -15369,7 +15367,7 @@
         <v>-3.8570000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>-9.4710000000000003E-3</v>
       </c>
@@ -15476,7 +15474,7 @@
         <v>-3.7780000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-8.8470000000000007E-3</v>
       </c>
@@ -15583,7 +15581,7 @@
         <v>-3.908E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>-8.4019999999999997E-3</v>
       </c>
@@ -15690,7 +15688,7 @@
         <v>-3.8609999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-7.5960000000000003E-3</v>
       </c>
@@ -15797,7 +15795,7 @@
         <v>-3.7320000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-7.1190000000000003E-3</v>
       </c>
@@ -15904,7 +15902,7 @@
         <v>-3.8119999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-6.5079999999999999E-3</v>
       </c>
@@ -16011,7 +16009,7 @@
         <v>-3.8159999999999999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-5.9249999999999997E-3</v>
       </c>
@@ -16118,7 +16116,7 @@
         <v>-3.7580000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-5.1320000000000003E-3</v>
       </c>
@@ -16225,7 +16223,7 @@
         <v>-3.6679999999999998E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-4.8580000000000003E-3</v>
       </c>
@@ -16332,7 +16330,7 @@
         <v>-3.5309999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>-4.9160000000000002E-3</v>
       </c>
@@ -16439,7 +16437,7 @@
         <v>-3.421E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>-5.2449999999999997E-3</v>
       </c>
@@ -16546,7 +16544,7 @@
         <v>-3.2940000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>-5.8999999999999999E-3</v>
       </c>
@@ -16653,7 +16651,7 @@
         <v>-3.0309999999999998E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-6.7629999999999999E-3</v>
       </c>
@@ -16760,7 +16758,7 @@
         <v>-2.8449999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-7.8220000000000008E-3</v>
       </c>
@@ -16867,7 +16865,7 @@
         <v>-2.6319999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-8.6490000000000004E-3</v>
       </c>
@@ -16974,7 +16972,7 @@
         <v>-2.4719999999999998E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-9.639E-3</v>
       </c>
@@ -17081,7 +17079,7 @@
         <v>-2.3349999999999998E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-9.6080000000000002E-3</v>
       </c>
@@ -17188,7 +17186,7 @@
         <v>-1.536E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-9.6089999999999995E-3</v>
       </c>
@@ -17295,7 +17293,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>-9.2999999999999992E-3</v>
       </c>
@@ -17402,7 +17400,7 @@
         <v>-1.469E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>-8.9479999999999994E-3</v>
       </c>
@@ -17509,7 +17507,7 @@
         <v>-1.4809999999999999E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-9.0410000000000004E-3</v>
       </c>
@@ -17616,7 +17614,7 @@
         <v>-1.5330000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-8.6440000000000006E-3</v>
       </c>
@@ -17723,7 +17721,7 @@
         <v>-1.555E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-8.4069999999999995E-3</v>
       </c>
@@ -17830,7 +17828,7 @@
         <v>-1.66E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-8.2459999999999999E-3</v>
       </c>
@@ -17937,7 +17935,7 @@
         <v>-1.7489999999999999E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-8.064E-3</v>
       </c>
@@ -18044,7 +18042,7 @@
         <v>-1.7750000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-8.2019999999999992E-3</v>
       </c>
@@ -18151,7 +18149,7 @@
         <v>-1.8450000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-8.0560000000000007E-3</v>
       </c>
@@ -18258,7 +18256,7 @@
         <v>-1.902E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-7.9369999999999996E-3</v>
       </c>
@@ -18365,7 +18363,7 @@
         <v>-1.933E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-7.9690000000000004E-3</v>
       </c>
@@ -18472,7 +18470,7 @@
         <v>-1.97E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-7.7330000000000003E-3</v>
       </c>
@@ -18579,7 +18577,7 @@
         <v>-2.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>-7.7270000000000004E-3</v>
       </c>
@@ -18686,7 +18684,7 @@
         <v>-2.055E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-7.705E-3</v>
       </c>
@@ -18793,7 +18791,7 @@
         <v>-2.088E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>-7.4609999999999998E-3</v>
       </c>
@@ -18900,7 +18898,7 @@
         <v>-2.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-7.3410000000000003E-3</v>
       </c>
@@ -19007,7 +19005,7 @@
         <v>-2.1619999999999999E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-7.3309999999999998E-3</v>
       </c>
@@ -19114,7 +19112,7 @@
         <v>-2.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-7.1980000000000004E-3</v>
       </c>
@@ -19221,7 +19219,7 @@
         <v>-2.1710000000000002E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-7.2509999999999996E-3</v>
       </c>
@@ -19328,7 +19326,7 @@
         <v>-2.2599999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>-7.1089999999999999E-3</v>
       </c>
@@ -19435,7 +19433,7 @@
         <v>-2.2799999999999999E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>-6.8580000000000004E-3</v>
       </c>
@@ -19542,7 +19540,7 @@
         <v>-2.3530000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-6.986E-3</v>
       </c>
@@ -19649,7 +19647,7 @@
         <v>-2.4290000000000002E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-6.9249999999999997E-3</v>
       </c>
@@ -19756,7 +19754,7 @@
         <v>-2.5379999999999999E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-6.7470000000000004E-3</v>
       </c>
@@ -19863,7 +19861,7 @@
         <v>-2.5509999999999999E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-6.8209999999999998E-3</v>
       </c>
@@ -19970,7 +19968,7 @@
         <v>-2.6580000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-6.6490000000000004E-3</v>
       </c>
@@ -20077,7 +20075,7 @@
         <v>-2.6949999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>-6.4850000000000003E-3</v>
       </c>
@@ -20184,7 +20182,7 @@
         <v>-2.7950000000000002E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-6.3400000000000001E-3</v>
       </c>
@@ -20291,7 +20289,7 @@
         <v>-2.9629999999999999E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>-6.1980000000000004E-3</v>
       </c>
@@ -20398,7 +20396,7 @@
         <v>-2.9659999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-6.0150000000000004E-3</v>
       </c>
@@ -20505,7 +20503,7 @@
         <v>-2.9949999999999998E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-5.9810000000000002E-3</v>
       </c>
@@ -20612,7 +20610,7 @@
         <v>-3.068E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>-6.1799999999999997E-3</v>
       </c>
@@ -20719,7 +20717,7 @@
         <v>-3.0019999999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-6.1149999999999998E-3</v>
       </c>
@@ -20826,7 +20824,7 @@
         <v>-2.905E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>-6.5690000000000002E-3</v>
       </c>
@@ -20933,7 +20931,7 @@
         <v>-2.8839999999999998E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>-6.6020000000000002E-3</v>
       </c>
@@ -21040,7 +21038,7 @@
         <v>-2.7650000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-6.3099999999999996E-3</v>
       </c>
@@ -21147,7 +21145,7 @@
         <v>-2.6740000000000002E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>-6.2199999999999998E-3</v>
       </c>
@@ -21254,7 +21252,7 @@
         <v>-2.6849999999999999E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-5.9670000000000001E-3</v>
       </c>
@@ -21361,7 +21359,7 @@
         <v>-2.689E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-5.4429999999999999E-3</v>
       </c>
@@ -21468,7 +21466,7 @@
         <v>-2.6489999999999999E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-4.9690000000000003E-3</v>
       </c>
@@ -21575,7 +21573,7 @@
         <v>-2.761E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-5.0340000000000003E-3</v>
       </c>

</xml_diff>